<commit_message>
register product functionality implemented
</commit_message>
<xml_diff>
--- a/product-detail.xlsx
+++ b/product-detail.xlsx
@@ -4,61 +4,47 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13360" windowHeight="5840"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>code</t>
   </si>
   <si>
-    <t>shortDescription</t>
-  </si>
-  <si>
-    <t>longDescription</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>stockReceived</t>
-  </si>
-  <si>
-    <t>registrar</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>abc-efg</t>
-  </si>
-  <si>
-    <t>soumyak</t>
-  </si>
-  <si>
-    <t>NEW</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>ppp</t>
-  </si>
-  <si>
-    <t>npr</t>
-  </si>
-  <si>
-    <t>fgt-tyy</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>buyUnitPrice</t>
+  </si>
+  <si>
+    <t>suggestedUnitPrice</t>
+  </si>
+  <si>
+    <t>saree</t>
+  </si>
+  <si>
+    <t>Red Blue Silk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fancy Violet </t>
+  </si>
+  <si>
+    <t>Rust Silk</t>
+  </si>
+  <si>
+    <t>Banarasi</t>
   </si>
 </sst>
 </file>
@@ -105,9 +91,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,41 +404,35 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -461,22 +440,17 @@
         <v>19090</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2">
-        <v>88.66</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1500</v>
       </c>
       <c r="E2" s="1">
-        <v>43845</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
+        <f>D2+D2*0.25</f>
+        <v>1875</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -484,22 +458,17 @@
         <v>19091</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4546</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>300</v>
       </c>
       <c r="E3" s="1">
-        <v>43846</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
+        <f t="shared" ref="E3:E5" si="0">D3+D3*0.25</f>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -507,22 +476,17 @@
         <v>19092</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2">
-        <v>6767</v>
+      <c r="D4" s="1">
+        <v>850</v>
       </c>
       <c r="E4" s="1">
-        <v>43847</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>1062.5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -530,184 +494,46 @@
         <v>19093</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2">
-        <v>825</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3000</v>
       </c>
       <c r="E5" s="1">
-        <v>43848</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>3750</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>19094</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2">
-        <v>456</v>
-      </c>
-      <c r="E6" s="1">
-        <v>43849</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>19095</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5665</v>
-      </c>
-      <c r="E7" s="1">
-        <v>43850</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>19096</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2">
-        <v>8898</v>
-      </c>
-      <c r="E8" s="1">
-        <v>43851</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>19097</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2">
-        <v>888</v>
-      </c>
-      <c r="E9" s="1">
-        <v>43852</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>19098</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2">
-        <v>122</v>
-      </c>
-      <c r="E10" s="1">
-        <v>43853</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>19099</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1">
-        <v>43854</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>19100</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="2">
-        <v>4546</v>
-      </c>
-      <c r="E12" s="1">
-        <v>43855</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented register product and sales
</commit_message>
<xml_diff>
--- a/product-detail.xlsx
+++ b/product-detail.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -401,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -418,7 +417,7 @@
     <col min="7" max="7" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -435,7 +434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>19090</v>
       </c>
@@ -453,7 +452,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>19091</v>
       </c>
@@ -471,7 +470,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>19092</v>
       </c>
@@ -489,7 +488,7 @@
         <v>1062.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>19093</v>
       </c>
@@ -507,33 +506,9 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>